<commit_message>
first draft of consumables, the ruby/yml file to format it, and the .odg for printing
</commit_message>
<xml_diff>
--- a/tactile_tabletop/Consumable Cards/Tactile_Tabletop_Data-Consumables.xlsx
+++ b/tactile_tabletop/Consumable Cards/Tactile_Tabletop_Data-Consumables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\TableTopRolePlaying_Squib\tactile_tabletop\Consumable Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBC0413-59E6-4036-83B9-0F1DEC9BD112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D924569-3C87-4AA4-83DB-9F4608096828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tactile Tabletop Data - Level 1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="174">
   <si>
     <t>Lunging Strike</t>
   </si>
@@ -380,28 +380,169 @@
     <t>Consumable Name</t>
   </si>
   <si>
-    <t>health potion</t>
-  </si>
-  <si>
-    <t>random stuff</t>
-  </si>
-  <si>
     <t>Consumable Variables</t>
   </si>
   <si>
     <t>Consumable Rules</t>
   </si>
   <si>
-    <t>X = 5</t>
-  </si>
-  <si>
-    <t>Y = d20</t>
-  </si>
-  <si>
-    <t>Restore X health</t>
-  </si>
-  <si>
-    <t>Y amount of random stuff you'd find in a pocket small rock, small strand of string, fluff, dirt)</t>
+    <t>Large Quartz Gem</t>
+  </si>
+  <si>
+    <t>Consumable Cost</t>
+  </si>
+  <si>
+    <t>Rope</t>
+  </si>
+  <si>
+    <t>reflective (2 inch round surface), and verr pretti</t>
+  </si>
+  <si>
+    <t>Wooden Pole</t>
+  </si>
+  <si>
+    <t>Rubber Wedge</t>
+  </si>
+  <si>
+    <t>30 feet of rope! Made of hemp. Odorless, impregnable, and coil-able!</t>
+  </si>
+  <si>
+    <t>10 feet long! Can be in 2 or 3 segment: either side has internal threading or pegs that can interface with the threading. 1in diameter, and super strong!</t>
+  </si>
+  <si>
+    <t>can keep a door open, no matter its weight! As long as that weight is less than about 40 points</t>
+  </si>
+  <si>
+    <t>Magnet</t>
+  </si>
+  <si>
+    <t>Detects the existence of all metals! Every one! There is no metal that this magnet can't detect!</t>
+  </si>
+  <si>
+    <t>Matchsticks</t>
+  </si>
+  <si>
+    <t>10 of them, They can start a small flame. A flame that's small. Not big. Unless you're not careful! :o</t>
+  </si>
+  <si>
+    <t>Firewood</t>
+  </si>
+  <si>
+    <t>a bunch of logs, they're pretty heavy because they are actually a bunch of firewood.</t>
+  </si>
+  <si>
+    <t>Hatchet</t>
+  </si>
+  <si>
+    <t>Spare knife</t>
+  </si>
+  <si>
+    <t xml:space="preserve">can be used as a weak hand weapon (1d4, Close range), but otherwise can cut rope, scour a painting, threaten an unarmed person, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">a short weapon (1d6, 5ft range), but otherwise can cut up plants (+3), turn wood into firewood, can be wielded menacingly, </t>
+  </si>
+  <si>
+    <t>Paint Bucket</t>
+  </si>
+  <si>
+    <t>Coat something in a color! Makes things easier to see, or identify compared to others. Also verr pretti!</t>
+  </si>
+  <si>
+    <t>Small Health Potion</t>
+  </si>
+  <si>
+    <t>a glass vial the size of a thumb, full of a deep red liquid. Heals 1d4+3 health immediately</t>
+  </si>
+  <si>
+    <t>Medium Health Potion</t>
+  </si>
+  <si>
+    <t>Large Health Potion</t>
+  </si>
+  <si>
+    <t>a glass vial the size of 2 thumbs, full of a deep reed liquid. Heals 2d4+6 immediately, reduces next die roll by 2</t>
+  </si>
+  <si>
+    <t>a glass vial the size of 3 thumbs, full of a deep reeed liquid. Heals 3d4+9 immediately, reduces next die roll by 8</t>
+  </si>
+  <si>
+    <t>When you need to [REDACTED] the [REDACTED]. Pretty hefty, but you can throw them ~30 feet, does 2d4 damage that then does 1d4 after a round.</t>
+  </si>
+  <si>
+    <t>Molotov Cocktail</t>
+  </si>
+  <si>
+    <t>Teleportation Stone</t>
+  </si>
+  <si>
+    <t>Don't ask where I got this. You can set your new location to anywhere within 30 feet, but because of the nausea your next die roll is -2</t>
+  </si>
+  <si>
+    <t>Odachi</t>
+  </si>
+  <si>
+    <t>Lazer Gun</t>
+  </si>
+  <si>
+    <t>Long Gun</t>
+  </si>
+  <si>
+    <t>yunno, guns? It's a longer one of those, with enough ammunition that you won't have to worry about it. This one does an extra d8 instead of a d6 at +30ft</t>
+  </si>
+  <si>
+    <t>Killer YoYo</t>
+  </si>
+  <si>
+    <t>&lt;Pretend Squib handled Japanese text and I put "Hey Skyler" here&gt; (great weapon). If you deal 5 damage, then enemy takes 1d4 additional damage at the end of their turn</t>
+  </si>
+  <si>
+    <t>Can be charged for a bigger blast, though it's hard to wield often this way (Great Castor). Add 4 damage instead of 3 for each type token on an enemy</t>
+  </si>
+  <si>
+    <t>a sick yoyo, with fire decals and neon yellow highlights (Reach Weapon). When thrown, explodes and deals the thrown damage in a 5ft area</t>
+  </si>
+  <si>
+    <t>Gauntlets of Ki Blast</t>
+  </si>
+  <si>
+    <t>Hold your fist aloft to send a medium range blast (Short Shot Weapon), and increase your health by 2</t>
+  </si>
+  <si>
+    <t>By drawing a sigil in the air, you can launch a blast of energy (Hand Castor). You can draw one symbol (at a time) that suspends in the air withstanding 500 pounds of force (can hold close a door, aid in climbing, etc.)</t>
+  </si>
+  <si>
+    <t>A Mighty Pen</t>
+  </si>
+  <si>
+    <t>Troublesome Sword</t>
+  </si>
+  <si>
+    <t>This sword (Short Weapon) has a hardened glass bubble in the hilt. Can re-roll a 1 or a 2 once per attack roll</t>
+  </si>
+  <si>
+    <t>Steely Resolve</t>
+  </si>
+  <si>
+    <t>With a gesture, you can brace your arm and to deflect incoming damage (Blocking Weapon). More than just being cool, once per combat you can get a +3 to an influence roll</t>
+  </si>
+  <si>
+    <t>Ring of Infinite Strike, level 1</t>
+  </si>
+  <si>
+    <t>A legendary ring granting improved punches (Hand Weapon). Damage is 1d4+1</t>
+  </si>
+  <si>
+    <t>Book of Puns/Jokes</t>
+  </si>
+  <si>
+    <t>Puns so bad, and jokes so good, you'll be the maestro of the party (Utility Weapon). Return an ally's card every turn instead of 50% of the time, and increase damage from this weapon by +2</t>
+  </si>
+  <si>
+    <t>Instant Pit</t>
+  </si>
+  <si>
+    <t>looks like a normal coin, but when thrown on the ground will instantly create a 10 ft deep pit. Only lasts for a few seconds (1 round), but sends whatever is at the bottom upwards!</t>
   </si>
 </sst>
 </file>
@@ -893,12 +1034,14 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1254,73 +1397,338 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F6:F8"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="38.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" style="3" customWidth="1"/>
-    <col min="8" max="8" width="34.85546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="30.28515625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="38.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" style="4" customWidth="1"/>
+    <col min="8" max="8" width="34.85546875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="30.28515625" style="4" customWidth="1"/>
     <col min="10" max="10" width="30.42578125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="21.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="7.85546875" style="3" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" style="3" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" style="3" customWidth="1"/>
-    <col min="16" max="16" width="45.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.42578125" style="3" customWidth="1"/>
-    <col min="18" max="18" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.7109375" style="3" customWidth="1"/>
-    <col min="20" max="20" width="33.140625" style="3" customWidth="1"/>
-    <col min="21" max="21" width="44.42578125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="21.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="7.85546875" style="4" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" style="4" customWidth="1"/>
+    <col min="15" max="15" width="18.28515625" style="4" customWidth="1"/>
+    <col min="16" max="16" width="45.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.42578125" style="4" customWidth="1"/>
+    <col min="18" max="18" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" style="4" customWidth="1"/>
+    <col min="20" max="20" width="33.140625" style="4" customWidth="1"/>
+    <col min="21" max="21" width="44.42578125" style="4" customWidth="1"/>
     <col min="22" max="22" width="43.42578125" style="4" customWidth="1"/>
-    <col min="23" max="16384" width="22.28515625" style="3"/>
+    <col min="23" max="16384" width="22.28515625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="J1" s="3"/>
-      <c r="V1" s="3"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C3" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>126</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D13" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D14" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D16" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D18" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D19" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D20" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D21" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D22" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D23" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D24" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D25" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D26" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D27" s="4">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1544,7 +1952,7 @@
       <c r="A23" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="2" t="s">
         <v>86</v>
       </c>
       <c r="C23" t="s">
@@ -1665,7 +2073,7 @@
       <c r="A37" t="s">
         <v>63</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C37" t="s">
@@ -1687,13 +2095,13 @@
       <c r="A39" t="s">
         <v>51</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="2" t="s">
         <v>52</v>
       </c>
       <c r="C39" t="s">
         <v>34</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" s="2" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1701,7 +2109,7 @@
       <c r="A40" t="s">
         <v>35</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C40" t="s">

</xml_diff>